<commit_message>
Admin console now created and ready to go ....
</commit_message>
<xml_diff>
--- a/DatabaseIndividualPricingInputFormat v2.xlsx
+++ b/DatabaseIndividualPricingInputFormat v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://redbrickza.sharepoint.com/sites/Empores/Shared Documents/NovaPower/Web Pricing Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{1A61F79C-627C-4E16-B2D7-902F4270E39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D98D6001-C139-4B50-B629-AF09A1BCD908}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{1A61F79C-627C-4E16-B2D7-902F4270E39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCC73803-DA10-4664-9CCD-04D8A37900C4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A38C0819-823B-4194-AA2B-5033FF66305C}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="186">
   <si>
     <t>ItemName</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>SizeGroup:6,TypeGroup:1, Brand:1, PackageGroup:1</t>
+  </si>
+  <si>
+    <t>https://thecoolguys.co.za/wp-content/uploads/2022/03/3kva-1.png</t>
   </si>
   <si>
     <t>Size-kVA:5, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:5, BatVoltage-V:48, MPPTVoltage-VDC:115</t>
@@ -1087,8 +1090,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45:H52"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -2090,6 +2093,9 @@
       <c r="G38" s="6" t="s">
         <v>94</v>
       </c>
+      <c r="H38" s="21" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="15">
       <c r="A39" s="6" t="s">
@@ -2105,7 +2111,7 @@
         <v>77</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F39" s="7">
         <f>RBCPriceGenerator!B42</f>
@@ -2114,6 +2120,9 @@
       <c r="G39" s="6" t="s">
         <v>94</v>
       </c>
+      <c r="H39" s="21" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="15">
       <c r="A40" s="6" t="s">
@@ -2126,17 +2135,20 @@
         <v>92</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F40" s="7">
         <f>RBCPriceGenerator!B43</f>
         <v>19544.25</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="H40" s="21" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15">
@@ -2150,17 +2162,20 @@
         <v>92</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F41" s="7">
         <f>RBCPriceGenerator!B44</f>
         <v>26449.999999999996</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15">
@@ -2174,17 +2189,20 @@
         <v>92</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F42" s="7">
         <f>RBCPriceGenerator!B45</f>
         <v>27542.499999999996</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15">
@@ -2198,17 +2216,20 @@
         <v>92</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F43" s="7">
         <f>RBCPriceGenerator!B46</f>
         <v>34477</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15">
@@ -2219,13 +2240,13 @@
         <v>75</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F44" s="9">
         <f>RBCPriceGenerator!B47</f>
@@ -2235,7 +2256,7 @@
         <v>94</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15">
@@ -2246,23 +2267,23 @@
         <v>75</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>81</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F45" s="9">
         <f>RBCPriceGenerator!B48</f>
         <v>4401.0499999999993</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15">
@@ -2273,13 +2294,13 @@
         <v>75</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F46" s="9">
         <f>RBCPriceGenerator!B49</f>
@@ -2289,7 +2310,7 @@
         <v>31</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15">
@@ -2300,13 +2321,13 @@
         <v>75</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F47" s="9">
         <f>RBCPriceGenerator!B50</f>
@@ -2316,7 +2337,7 @@
         <v>94</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15">
@@ -2327,23 +2348,23 @@
         <v>75</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>81</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F48" s="9">
         <f>RBCPriceGenerator!B51</f>
         <v>17480</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H48" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15">
@@ -2354,23 +2375,23 @@
         <v>75</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F49" s="9">
         <f>RBCPriceGenerator!B55</f>
         <v>15864.249999999998</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15">
@@ -2381,23 +2402,23 @@
         <v>75</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F50" s="9">
         <f>RBCPriceGenerator!B56</f>
         <v>40340.85</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15">
@@ -2408,23 +2429,23 @@
         <v>75</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F51" s="9">
         <f>RBCPriceGenerator!B57</f>
         <v>48275.85</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15">
@@ -2435,23 +2456,23 @@
         <v>75</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F52" s="9">
         <f>RBCPriceGenerator!B58</f>
         <v>67286.5</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H52" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15">
@@ -2462,20 +2483,20 @@
         <v>75</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F53" s="2">
         <f>RBCPriceGenerator!B59</f>
         <v>14614.199999999999</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15">
@@ -2486,20 +2507,20 @@
         <v>75</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F54" s="2">
         <f>RBCPriceGenerator!B60</f>
         <v>16660.05</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15">
@@ -2510,20 +2531,20 @@
         <v>75</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F55" s="2">
         <f>RBCPriceGenerator!B61</f>
         <v>27958.799999999999</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15">
@@ -2534,20 +2555,20 @@
         <v>75</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F56" s="2">
         <f>RBCPriceGenerator!B62</f>
         <v>6481.4</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15">
@@ -2558,20 +2579,20 @@
         <v>75</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F57" s="2">
         <f>RBCPriceGenerator!B63</f>
         <v>8204.0999999999985</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15">
@@ -2582,20 +2603,20 @@
         <v>75</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F58" s="2">
         <f>RBCPriceGenerator!B64</f>
         <v>13881.65</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="5" customFormat="1" ht="15">
@@ -2606,20 +2627,20 @@
         <v>75</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F59" s="2">
         <f>RBCPriceGenerator!B65</f>
         <v>15917.15</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H59" s="19"/>
     </row>
@@ -2631,20 +2652,20 @@
         <v>75</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F60" s="2">
         <f>RBCPriceGenerator!B66</f>
         <v>26767.399999999998</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H60" s="19"/>
     </row>
@@ -2656,20 +2677,20 @@
         <v>75</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F61" s="12">
         <f>RBCPriceGenerator!B70</f>
         <v>10804.25</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H61" s="19"/>
     </row>
@@ -2681,20 +2702,20 @@
         <v>75</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F62" s="12">
         <f>RBCPriceGenerator!B71</f>
         <v>11034.25</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H62" s="19"/>
     </row>
@@ -2706,20 +2727,20 @@
         <v>75</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F63" s="12">
         <f>RBCPriceGenerator!B72</f>
         <v>21154.25</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H63" s="19"/>
     </row>
@@ -2731,38 +2752,38 @@
         <v>75</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F64" s="12">
         <f>RBCPriceGenerator!B73</f>
         <v>25288.499999999996</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H64" s="19"/>
     </row>
     <row r="65" spans="1:8" s="5" customFormat="1" ht="15" hidden="1" thickBot="1">
       <c r="A65" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B65" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C65" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D65" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E65" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F65" s="14">
         <f>RBCPriceGenerator!B13</f>
@@ -2774,19 +2795,19 @@
     </row>
     <row r="66" spans="1:8" s="5" customFormat="1" ht="15" hidden="1" thickBot="1">
       <c r="A66" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D66" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E66" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F66" s="14">
         <f>RBCPriceGenerator!B14</f>
@@ -2798,19 +2819,19 @@
     </row>
     <row r="67" spans="1:8" ht="15" hidden="1" thickBot="1">
       <c r="A67" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D67" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E67" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F67" s="14">
         <f>RBCPriceGenerator!B15</f>
@@ -2823,19 +2844,19 @@
     </row>
     <row r="68" spans="1:8" ht="15" hidden="1" thickBot="1">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D68" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E68" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F68" s="14">
         <f>RBCPriceGenerator!B16</f>
@@ -2848,19 +2869,19 @@
     </row>
     <row r="69" spans="1:8" ht="15" hidden="1" thickBot="1">
       <c r="A69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C69" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D69" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E69" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F69" s="14">
         <f>RBCPriceGenerator!B17</f>
@@ -2873,19 +2894,19 @@
     </row>
     <row r="70" spans="1:8" ht="15" hidden="1" thickBot="1">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D70" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E70" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F70" s="14">
         <f>RBCPriceGenerator!B18</f>
@@ -2898,82 +2919,82 @@
     </row>
     <row r="71" spans="1:8" ht="15" hidden="1" thickBot="1">
       <c r="A71" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F71" s="2">
         <f>RBCPriceGenerator!B67</f>
         <v>35255.549999999996</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H71"/>
     </row>
     <row r="72" spans="1:8" ht="15" hidden="1" thickBot="1">
       <c r="A72" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F72" s="2">
         <f>RBCPriceGenerator!B68</f>
         <v>44369.299999999996</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H72"/>
     </row>
     <row r="73" spans="1:8" ht="15" hidden="1" thickBot="1">
       <c r="A73" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F73" s="2">
         <f>RBCPriceGenerator!B69</f>
         <v>45158.2</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H73"/>
     </row>
     <row r="74" spans="1:8" ht="15" hidden="1" thickBot="1">
       <c r="C74" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F74" s="12">
         <f>RBCPriceGenerator!B74</f>
@@ -3212,6 +3233,8 @@
   <hyperlinks>
     <hyperlink ref="H45" r:id="rId1" xr:uid="{5AC0C6E4-66C8-46E6-80A8-12658489C699}"/>
     <hyperlink ref="H46:H52" r:id="rId2" display="https://i.ibb.co/N2BqyKx/Rentech-5-6.png" xr:uid="{0AE3E508-AADC-4871-B8E8-A8BE2D77B813}"/>
+    <hyperlink ref="H38" r:id="rId3" xr:uid="{7E430A18-0B09-47BD-8436-95CDF5D784DB}"/>
+    <hyperlink ref="H39:H43" r:id="rId4" display="https://thecoolguys.co.za/wp-content/uploads/2022/03/3kva-1.png" xr:uid="{A68A78BA-2918-4268-9449-0F7F842D2D78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4159,7 +4182,7 @@
         <v>77</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F39" s="7">
         <f>RBCPriceGenerator!B42</f>
@@ -4180,17 +4203,17 @@
         <v>92</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F40" s="7">
         <f>RBCPriceGenerator!B43</f>
         <v>19544.25</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1">
@@ -4204,17 +4227,17 @@
         <v>92</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F41" s="7">
         <f>RBCPriceGenerator!B44</f>
         <v>26449.999999999996</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1">
@@ -4228,17 +4251,17 @@
         <v>92</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F42" s="7">
         <f>RBCPriceGenerator!B45</f>
         <v>27542.499999999996</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1">
@@ -4252,17 +4275,17 @@
         <v>92</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F43" s="7">
         <f>RBCPriceGenerator!B46</f>
         <v>34477</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1">
@@ -4273,13 +4296,13 @@
         <v>75</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F44" s="9">
         <f>RBCPriceGenerator!B47</f>
@@ -4297,20 +4320,20 @@
         <v>75</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>81</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F45" s="9">
         <f>RBCPriceGenerator!B48</f>
         <v>4401.0499999999993</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1">
@@ -4321,13 +4344,13 @@
         <v>75</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F46" s="9">
         <f>RBCPriceGenerator!B49</f>
@@ -4345,13 +4368,13 @@
         <v>75</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F47" s="9">
         <f>RBCPriceGenerator!B50</f>
@@ -4369,20 +4392,20 @@
         <v>75</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>81</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F48" s="9">
         <f>RBCPriceGenerator!B51</f>
         <v>17480</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1">
@@ -4393,20 +4416,20 @@
         <v>75</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F49" s="9">
         <f>RBCPriceGenerator!B55</f>
         <v>15864.249999999998</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1">
@@ -4417,20 +4440,20 @@
         <v>75</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F50" s="9">
         <f>RBCPriceGenerator!B56</f>
         <v>40340.85</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1">
@@ -4441,20 +4464,20 @@
         <v>75</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F51" s="9">
         <f>RBCPriceGenerator!B57</f>
         <v>48275.85</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" thickBot="1">
@@ -4465,20 +4488,20 @@
         <v>75</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F52" s="9">
         <f>RBCPriceGenerator!B58</f>
         <v>67286.5</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1">
@@ -4489,20 +4512,20 @@
         <v>75</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F53" s="2">
         <f>RBCPriceGenerator!B59</f>
         <v>14614.199999999999</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" thickBot="1">
@@ -4513,20 +4536,20 @@
         <v>75</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F54" s="2">
         <f>RBCPriceGenerator!B60</f>
         <v>16660.05</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1">
@@ -4537,20 +4560,20 @@
         <v>75</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F55" s="2">
         <f>RBCPriceGenerator!B61</f>
         <v>27958.799999999999</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15" thickBot="1">
@@ -4561,20 +4584,20 @@
         <v>75</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F56" s="2">
         <f>RBCPriceGenerator!B62</f>
         <v>6481.4</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1">
@@ -4585,20 +4608,20 @@
         <v>75</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F57" s="2">
         <f>RBCPriceGenerator!B63</f>
         <v>8204.0999999999985</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1">
@@ -4609,20 +4632,20 @@
         <v>75</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F58" s="2">
         <f>RBCPriceGenerator!B64</f>
         <v>13881.65</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1">
@@ -4633,20 +4656,20 @@
         <v>75</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F59" s="2">
         <f>RBCPriceGenerator!B65</f>
         <v>15917.15</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1">
@@ -4657,20 +4680,20 @@
         <v>75</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F60" s="2">
         <f>RBCPriceGenerator!B66</f>
         <v>26767.399999999998</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1">
@@ -4681,20 +4704,20 @@
         <v>75</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F61" s="12">
         <f>RBCPriceGenerator!B70</f>
         <v>10804.25</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1">
@@ -4705,20 +4728,20 @@
         <v>75</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F62" s="12">
         <f>RBCPriceGenerator!B71</f>
         <v>11034.25</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1">
@@ -4729,20 +4752,20 @@
         <v>75</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F63" s="12">
         <f>RBCPriceGenerator!B72</f>
         <v>21154.25</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:7" s="5" customFormat="1" ht="15" thickBot="1">
@@ -4753,37 +4776,37 @@
         <v>75</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F64" s="12">
         <f>RBCPriceGenerator!B73</f>
         <v>25288.499999999996</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:7" s="5" customFormat="1" ht="15" hidden="1" thickBot="1">
       <c r="A65" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B65" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C65" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D65" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E65" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F65" s="14">
         <f>RBCPriceGenerator!B13</f>
@@ -4795,19 +4818,19 @@
     </row>
     <row r="66" spans="1:7" s="5" customFormat="1" ht="15" hidden="1" thickBot="1">
       <c r="A66" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D66" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E66" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F66" s="14">
         <f>RBCPriceGenerator!B14</f>
@@ -4819,19 +4842,19 @@
     </row>
     <row r="67" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A67" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D67" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E67" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F67" s="14">
         <f>RBCPriceGenerator!B15</f>
@@ -4843,19 +4866,19 @@
     </row>
     <row r="68" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D68" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E68" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F68" s="14">
         <f>RBCPriceGenerator!B16</f>
@@ -4867,19 +4890,19 @@
     </row>
     <row r="69" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C69" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D69" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E69" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F69" s="14">
         <f>RBCPriceGenerator!B17</f>
@@ -4891,19 +4914,19 @@
     </row>
     <row r="70" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D70" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E70" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F70" s="14">
         <f>RBCPriceGenerator!B18</f>
@@ -4915,79 +4938,79 @@
     </row>
     <row r="71" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A71" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F71" s="2">
         <f>RBCPriceGenerator!B67</f>
         <v>35255.549999999996</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A72" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F72" s="2">
         <f>RBCPriceGenerator!B68</f>
         <v>44369.299999999996</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="A73" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F73" s="2">
         <f>RBCPriceGenerator!B69</f>
         <v>45158.2</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="C74" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F74" s="12">
         <f>RBCPriceGenerator!B74</f>
@@ -5038,7 +5061,7 @@
         <v>10471.9</v>
       </c>
       <c r="G81" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -5067,7 +5090,7 @@
         <v>13549.3</v>
       </c>
       <c r="G82" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -5096,7 +5119,7 @@
         <v>15525</v>
       </c>
       <c r="G83" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -5134,7 +5157,7 @@
         <v>10471.9</v>
       </c>
       <c r="G86" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -5163,7 +5186,7 @@
         <v>27098.6</v>
       </c>
       <c r="G87" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -5192,7 +5215,7 @@
         <v>20700</v>
       </c>
       <c r="G88" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -5230,7 +5253,7 @@
         <v>15234.05</v>
       </c>
       <c r="G91" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -5259,7 +5282,7 @@
         <v>26444.249999999996</v>
       </c>
       <c r="G92" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -5288,7 +5311,7 @@
         <v>29071.999999999996</v>
       </c>
       <c r="G93" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -5329,7 +5352,7 @@
         <v>15234.05</v>
       </c>
       <c r="G97" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -5358,7 +5381,7 @@
         <v>52888.499999999993</v>
       </c>
       <c r="G98" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -5387,7 +5410,7 @@
         <v>36339.999999999993</v>
       </c>
       <c r="G99" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="100" spans="1:14">
@@ -5428,7 +5451,7 @@
         <v>41260.85</v>
       </c>
       <c r="G103" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="104" spans="1:14">
@@ -5457,7 +5480,7 @@
         <v>52888.499999999993</v>
       </c>
       <c r="G104" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="105" spans="1:14">
@@ -5486,7 +5509,7 @@
         <v>36339.999999999993</v>
       </c>
       <c r="G105" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" spans="1:14">
@@ -5519,7 +5542,7 @@
         <v>0</v>
       </c>
       <c r="N106" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="107" spans="1:14">
@@ -5549,7 +5572,7 @@
         <v>0</v>
       </c>
       <c r="N107" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:14">
@@ -5579,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="N108" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="109" spans="1:14">
@@ -5615,7 +5638,7 @@
         <v>41260.85</v>
       </c>
       <c r="G110" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M110" s="16"/>
     </row>
@@ -5645,7 +5668,7 @@
         <v>52888.499999999993</v>
       </c>
       <c r="G111" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H111">
         <f t="shared" ref="H111:I111" si="23">H$35</f>
@@ -5672,7 +5695,7 @@
         <v>0</v>
       </c>
       <c r="N111" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="112" spans="1:14">
@@ -5701,7 +5724,7 @@
         <v>43607.999999999993</v>
       </c>
       <c r="G112" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H112">
         <f>H$4</f>
@@ -5728,7 +5751,7 @@
         <v>0</v>
       </c>
       <c r="N112" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="113" spans="1:14">
@@ -5761,7 +5784,7 @@
         <v>0</v>
       </c>
       <c r="N113" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="114" spans="1:14">
@@ -5799,7 +5822,7 @@
         <v>0</v>
       </c>
       <c r="N116" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="117" spans="1:14">
@@ -5828,7 +5851,7 @@
         <v>41260.85</v>
       </c>
       <c r="G117" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H117">
         <f t="shared" ref="H117:K117" si="30">H$7</f>
@@ -5855,7 +5878,7 @@
         <v>0</v>
       </c>
       <c r="N117" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="118" spans="1:14">
@@ -5884,7 +5907,7 @@
         <v>79332.749999999985</v>
       </c>
       <c r="G118" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H118">
         <f t="shared" ref="H118:K118" si="32">H$70</f>
@@ -5911,7 +5934,7 @@
         <v>0</v>
       </c>
       <c r="N118" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="119" spans="1:14">
@@ -5940,7 +5963,7 @@
         <v>50875.999999999993</v>
       </c>
       <c r="G119" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="M119" s="16">
         <f>SUBTOTAL(9,M116:M118)</f>
@@ -5983,7 +6006,7 @@
         <v>0</v>
       </c>
       <c r="N122" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="123" spans="1:14">
@@ -6012,7 +6035,7 @@
         <v>0</v>
       </c>
       <c r="N123" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="124" spans="1:14">
@@ -6041,7 +6064,7 @@
         <v>0</v>
       </c>
       <c r="N124" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="125" spans="1:14">
@@ -6082,7 +6105,7 @@
         <v>0</v>
       </c>
       <c r="N128" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="129" spans="8:14">
@@ -6111,7 +6134,7 @@
         <v>0</v>
       </c>
       <c r="N129" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="130" spans="8:14">
@@ -6140,7 +6163,7 @@
         <v>0</v>
       </c>
       <c r="N130" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="131" spans="8:14">
@@ -6184,7 +6207,7 @@
         <v>0</v>
       </c>
       <c r="N135" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="136" spans="8:14">
@@ -6213,7 +6236,7 @@
         <v>0</v>
       </c>
       <c r="N136" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="137" spans="8:14">
@@ -6242,7 +6265,7 @@
         <v>0</v>
       </c>
       <c r="N137" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="138" spans="8:14">
@@ -6277,7 +6300,7 @@
         <v>0</v>
       </c>
       <c r="N142" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="143" spans="8:14">
@@ -6306,7 +6329,7 @@
         <v>0</v>
       </c>
       <c r="N143" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="144" spans="8:14">
@@ -6335,7 +6358,7 @@
         <v>0</v>
       </c>
       <c r="N144" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="145" spans="13:13">

</xml_diff>

<commit_message>
ready changes and stable release
</commit_message>
<xml_diff>
--- a/DatabaseIndividualPricingInputFormat v2.xlsx
+++ b/DatabaseIndividualPricingInputFormat v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://redbrickza-my.sharepoint.com/personal/ezekiel_mokaedi_rbconsult_co_za/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{397845D5-7D5E-44ED-BEA3-9292ED887155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{882A49D1-94E5-4E59-BCD6-2A82FC39189D}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{397845D5-7D5E-44ED-BEA3-9292ED887155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61E9067E-F322-402D-A8BB-D84881B41F77}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{A38C0819-823B-4194-AA2B-5033FF66305C}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Packages!$A$1:$G$57</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$G$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$G$27</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="186">
   <si>
     <t>ItemName</t>
   </si>
@@ -67,7 +67,7 @@
     <t>img_url</t>
   </si>
   <si>
-    <t>Product Description</t>
+    <t>Description</t>
   </si>
   <si>
     <t>Battery</t>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">https://i.ibb.co/9sXfd3v/Axitec370-W.png </t>
   </si>
   <si>
-    <t>s</t>
+    <t xml:space="preserve">https://i.ibb.co/zxCRs8d/Des-ORSpec-Axitec370-W.png </t>
   </si>
   <si>
     <t>JA Solar</t>
@@ -244,6 +244,9 @@
     <t>Size-kVA:7.5, EngineSize-Stroke: 4</t>
   </si>
   <si>
+    <t>https://i.ibb.co/42kmFyg/Petrol7-5k-VA-R14-9k.jpg</t>
+  </si>
+  <si>
     <t>Diesel</t>
   </si>
   <si>
@@ -253,220 +256,235 @@
     <t>Size-kVA:7, EngineSize-Stroke: 4</t>
   </si>
   <si>
+    <t>https://i.ibb.co/MPzRSq3/Diesel7k-VA-R27-6.png</t>
+  </si>
+  <si>
+    <t>Inverter</t>
+  </si>
+  <si>
+    <t>Inverters</t>
+  </si>
+  <si>
+    <t>Rentech-Axpert</t>
+  </si>
+  <si>
+    <t>Stand-alone</t>
+  </si>
+  <si>
+    <t>Size-kVA:5.6, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:5.6, BatVoltage-V:48</t>
+  </si>
+  <si>
+    <t>SizeGroup:5,TypeGroup:1, Brand:1, PackageGroup:1</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/FK0ty82/Tentech5-6k-VA-R17-4.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/rG3Z1KZ/Des-Rentech5-6k-VA-R17-4.png</t>
+  </si>
+  <si>
+    <t>Size-kVA:5.5, EngineSize-Stroke: 4</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/3SNsR9N/Petrol5-5k-VA-R13-8.jpg</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Size-kVA:5,InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:5, BatVoltage-V:48, MPPTCurrent-A:80</t>
+  </si>
+  <si>
+    <t>SizeGroup:6,TypeGroup:1, Brand:1, PackageGroup:1</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/Y0KkM3P/RCT-Axpert5k-VA-R15-7k.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/BGWST2R/Des-Rentech-Axpert5k-VA-R15-7.png</t>
+  </si>
+  <si>
+    <t>Mecer</t>
+  </si>
+  <si>
+    <t>Size-kVA:5, Voltage-V:48, Power-kW:4</t>
+  </si>
+  <si>
+    <t>SizeGroup:3,TypeGroup:1, Brand:1, PackageGroup:1</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/31W0tKZ/Mecer5k-VA-R12-8k.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/WHbWBfr/Des-Mecer5k-VA-R12-8.png</t>
+  </si>
+  <si>
+    <t>TheCoolGuys</t>
+  </si>
+  <si>
+    <t>Size-kVA:5, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:5, BatVoltage-V:48, MPPTVoltage-VDC:115</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/cNq40GD/TCG5k-VA-R16-1k.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/SwJ5vSF/Des-TCG5k-VA-R16-1.png</t>
+  </si>
+  <si>
+    <t>Size-kVA:3.5, EngineSize-Stroke: 4</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/4p6Tjxs/Petrol3-5-KVA-R8-0k.png</t>
+  </si>
+  <si>
+    <t>RCT-AXPERT</t>
+  </si>
+  <si>
+    <t>Size-kVA:3, Voltage-V:48, Power-kW:3, MPPTVoltage-V:430</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/n1CmNTS/RCT-Axpert3k-VA-R10-4k.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/wrF2yST/Spec-ORDes-RCT-AXPERT3k-VA-R10-4.png</t>
+  </si>
+  <si>
+    <t>Size-kVA:3, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:2.4, BatVoltage-V:24, MPPTVoltage-VDC:100</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/t25SQL4/TCG3kva-R8-6-K.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/zPN6ykP/Des-TCG3k-VA-R8-6.png</t>
+  </si>
+  <si>
+    <t>Size-kVA:3, EngineSize-Stroke: 4</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/SrqNKTT/Diesel3k-VA-R17-2.png</t>
+  </si>
+  <si>
+    <t>Rentech-Jagular</t>
+  </si>
+  <si>
+    <t>Size-kVA:2.4, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:1.4, RecLABatVoltage-V:12</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/6r0kNwc/Rentech-Jag2-4k-VA-R4-4k.png</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/MC08H1B/Des-Rentec-Jag2-4k-VA-R4-4k.png</t>
+  </si>
+  <si>
+    <t>Size-kVA:10, EngineSize-Stroke: 4</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/b16FBDs/Petrol10k-VA-65-6.jpg</t>
+  </si>
+  <si>
+    <t>Pull-Start</t>
+  </si>
+  <si>
+    <t>Size-kVA:1.2, EngineSize-Stroke: 4</t>
+  </si>
+  <si>
+    <t>https://i.ibb.co/VTVCC5V/Petrol1-2k-VA-R5-1k.png</t>
+  </si>
+  <si>
+    <t>ImageUrl</t>
+  </si>
+  <si>
+    <t>MaxLi</t>
+  </si>
+  <si>
+    <t>Voltage-V:12, Energy-kWh:1.2</t>
+  </si>
+  <si>
+    <t>Voltage-V:12, Energy-kWh:1.5</t>
+  </si>
+  <si>
+    <t>Fusion</t>
+  </si>
+  <si>
+    <t>Forbatt</t>
+  </si>
+  <si>
+    <t>Lead Acid</t>
+  </si>
+  <si>
+    <t>Voltage-V:12, Energy-kWh:1.2, Capacity-Ah:100</t>
+  </si>
+  <si>
+    <t>Deltec</t>
+  </si>
+  <si>
+    <t>Lead Calcium</t>
+  </si>
+  <si>
+    <t>Voltage-V:12, Energy-kWh:1.2, Capacity-Ah:105</t>
+  </si>
+  <si>
+    <t>Pylon</t>
+  </si>
+  <si>
+    <t>Voltage-V:48, Energy-kWh:3.5, DischargeVoltage-V:53.5, ChargeVoltage-V:53.5</t>
+  </si>
+  <si>
+    <t>RCT</t>
+  </si>
+  <si>
+    <t>Voltage-V:12, Energy-kWh:2.4, Capacity-Ah:200</t>
+  </si>
+  <si>
+    <t>Voltage-V:25.6, Energy-kWh:5.12, RechargeVoltage-V:27.6, Capacity-Ah:200</t>
+  </si>
+  <si>
+    <t>Cable</t>
+  </si>
+  <si>
+    <t>Geewiz</t>
+  </si>
+  <si>
+    <t>SingleCore-DC</t>
+  </si>
+  <si>
+    <t>Size-mm2:35, Length-m:1</t>
+  </si>
+  <si>
+    <t>Size-mm2:50, Length-m:1</t>
+  </si>
+  <si>
+    <t>Rack</t>
+  </si>
+  <si>
+    <t>Renusol</t>
+  </si>
+  <si>
+    <t>Mounting Rail</t>
+  </si>
+  <si>
+    <t>Length-m:2.1</t>
+  </si>
+  <si>
+    <t>SizeGroup:1,TypeGroup:1, Brand:1, PackageGroup:1</t>
+  </si>
+  <si>
+    <t>Length-m:4.2</t>
+  </si>
+  <si>
     <t>Talon</t>
   </si>
   <si>
     <t>Electric-Start</t>
   </si>
   <si>
+    <t>Size-kVA:6, EngineSize-Stroke: 4</t>
+  </si>
+  <si>
+    <t>Size-kVA:4.5, EngineSize-Stroke: 4</t>
+  </si>
+  <si>
     <t>Size-kVA:6.4, EngineSize-Stroke: 4</t>
-  </si>
-  <si>
-    <t>Size-kVA:6, EngineSize-Stroke: 4</t>
-  </si>
-  <si>
-    <t>Inverter</t>
-  </si>
-  <si>
-    <t>Inverters</t>
-  </si>
-  <si>
-    <t>Rentech-Axpert</t>
-  </si>
-  <si>
-    <t>Stand-alone</t>
-  </si>
-  <si>
-    <t>Size-kVA:5.6, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:5.6, BatVoltage-V:48</t>
-  </si>
-  <si>
-    <t>SizeGroup:5,TypeGroup:1, Brand:1, PackageGroup:1</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/FK0ty82/Tentech5-6k-VA-R17-4.png</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/rG3Z1KZ/Des-Rentech5-6k-VA-R17-4.png</t>
-  </si>
-  <si>
-    <t>Size-kVA:5.5, EngineSize-Stroke: 4</t>
-  </si>
-  <si>
-    <t>Hybrid</t>
-  </si>
-  <si>
-    <t>Size-kVA:5,InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:5, BatVoltage-V:48, MPPTCurrent-A:80</t>
-  </si>
-  <si>
-    <t>SizeGroup:6,TypeGroup:1, Brand:1, PackageGroup:1</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/Y0KkM3P/RCT-Axpert5k-VA-R15-7k.png</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/BGWST2R/Des-Rentech-Axpert5k-VA-R15-7.png</t>
-  </si>
-  <si>
-    <t>Mecer</t>
-  </si>
-  <si>
-    <t>Size-kVA:5, Voltage-V:48, Power-kW:4</t>
-  </si>
-  <si>
-    <t>SizeGroup:3,TypeGroup:1, Brand:1, PackageGroup:1</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/31W0tKZ/Mecer5k-VA-R12-8k.png</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/WHbWBfr/Des-Mecer5k-VA-R12-8.png</t>
-  </si>
-  <si>
-    <t>TheCoolGuys</t>
-  </si>
-  <si>
-    <t>Size-kVA:5, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:5, BatVoltage-V:48, MPPTVoltage-VDC:115</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/cNq40GD/TCG5k-VA-R16-1k.png</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/SwJ5vSF/Des-TCG5k-VA-R16-1.png</t>
-  </si>
-  <si>
-    <t>Size-kVA:4.5, EngineSize-Stroke: 4</t>
-  </si>
-  <si>
-    <t>Size-kVA:3.5, EngineSize-Stroke: 4</t>
-  </si>
-  <si>
-    <t>RCT-AXPERT</t>
-  </si>
-  <si>
-    <t>Size-kVA:3, Voltage-V:48, Power-kW:3, MPPTVoltage-V:430</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/n1CmNTS/RCT-Axpert3k-VA-R10-4k.png</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/wrF2yST/Spec-ORDes-RCT-AXPERT3k-VA-R10-4.png</t>
-  </si>
-  <si>
-    <t>Size-kVA:3, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:2.4, BatVoltage-V:24, MPPTVoltage-VDC:100</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/t25SQL4/TCG3kva-R8-6-K.png</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/zPN6ykP/Des-TCG3k-VA-R8-6.png</t>
-  </si>
-  <si>
-    <t>Size-kVA:3, EngineSize-Stroke: 4</t>
-  </si>
-  <si>
-    <t>Rentech-Jagular</t>
-  </si>
-  <si>
-    <t>Size-kVA:2.4, InputVoltage-AC:230, OutputVoltage-AC:230, Power-kW:1.4, RecLABatVoltage-V:12</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/6r0kNwc/Rentech-Jag2-4k-VA-R4-4k.png</t>
-  </si>
-  <si>
-    <t>https://i.ibb.co/MC08H1B/Des-Rentec-Jag2-4k-VA-R4-4k.png</t>
-  </si>
-  <si>
-    <t>Size-kVA:10, EngineSize-Stroke: 4</t>
-  </si>
-  <si>
-    <t>Pull-Start</t>
-  </si>
-  <si>
-    <t>Size-kVA:1.2, EngineSize-Stroke: 4</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>ImageUrl</t>
-  </si>
-  <si>
-    <t>MaxLi</t>
-  </si>
-  <si>
-    <t>Voltage-V:12, Energy-kWh:1.2</t>
-  </si>
-  <si>
-    <t>Voltage-V:12, Energy-kWh:1.5</t>
-  </si>
-  <si>
-    <t>Fusion</t>
-  </si>
-  <si>
-    <t>Forbatt</t>
-  </si>
-  <si>
-    <t>Lead Acid</t>
-  </si>
-  <si>
-    <t>Voltage-V:12, Energy-kWh:1.2, Capacity-Ah:100</t>
-  </si>
-  <si>
-    <t>Deltec</t>
-  </si>
-  <si>
-    <t>Lead Calcium</t>
-  </si>
-  <si>
-    <t>Voltage-V:12, Energy-kWh:1.2, Capacity-Ah:105</t>
-  </si>
-  <si>
-    <t>Pylon</t>
-  </si>
-  <si>
-    <t>Voltage-V:48, Energy-kWh:3.5, DischargeVoltage-V:53.5, ChargeVoltage-V:53.5</t>
-  </si>
-  <si>
-    <t>RCT</t>
-  </si>
-  <si>
-    <t>Voltage-V:12, Energy-kWh:2.4, Capacity-Ah:200</t>
-  </si>
-  <si>
-    <t>Voltage-V:25.6, Energy-kWh:5.12, RechargeVoltage-V:27.6, Capacity-Ah:200</t>
-  </si>
-  <si>
-    <t>Cable</t>
-  </si>
-  <si>
-    <t>Geewiz</t>
-  </si>
-  <si>
-    <t>SingleCore-DC</t>
-  </si>
-  <si>
-    <t>Size-mm2:35, Length-m:1</t>
-  </si>
-  <si>
-    <t>Size-mm2:50, Length-m:1</t>
-  </si>
-  <si>
-    <t>Rack</t>
-  </si>
-  <si>
-    <t>Renusol</t>
-  </si>
-  <si>
-    <t>Mounting Rail</t>
-  </si>
-  <si>
-    <t>Length-m:2.1</t>
-  </si>
-  <si>
-    <t>SizeGroup:1,TypeGroup:1, Brand:1, PackageGroup:1</t>
-  </si>
-  <si>
-    <t>Length-m:4.2</t>
   </si>
   <si>
     <t>Size-kVA:1.5, Voltage-V:12, Power-kW:1.2</t>
@@ -1045,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BCF050-2F09-42D0-9049-6BF8B00124F4}">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1476,22 +1494,25 @@
       <c r="G14" t="s">
         <v>14</v>
       </c>
+      <c r="H14" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1">
       <c r="A15" t="s">
         <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D15" t="s">
         <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F15" s="13">
         <f>RBCPriceGenerator!B30</f>
@@ -1500,37 +1521,46 @@
       <c r="G15" t="s">
         <v>14</v>
       </c>
+      <c r="H15" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="15" thickBot="1">
-      <c r="A16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="13">
-        <f>RBCPriceGenerator!B31</f>
-        <v>32996.949999999997</v>
-      </c>
-      <c r="G16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="5" customFormat="1" ht="15" thickBot="1">
+      <c r="A16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="9">
+        <f>RBCPriceGenerator!B51</f>
+        <v>17480</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="A17" t="s">
         <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>64</v>
@@ -1539,183 +1569,194 @@
         <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F17" s="13">
-        <f>RBCPriceGenerator!B33</f>
-        <v>41400</v>
+        <f>RBCPriceGenerator!B25</f>
+        <v>13799.999999999998</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
-      <c r="H17"/>
+      <c r="H17" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15" thickBot="1">
-      <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="A18" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="13">
-        <f>RBCPriceGenerator!B29</f>
-        <v>27706.949999999997</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1">
-      <c r="A19" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="9">
-        <f>RBCPriceGenerator!B51</f>
-        <v>17480</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
-      <c r="A20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D18" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="13">
-        <f>RBCPriceGenerator!B25</f>
-        <v>13799.999999999998</v>
-      </c>
-      <c r="G20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1">
-      <c r="A21" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" s="9">
+      <c r="F18" s="9">
         <f>RBCPriceGenerator!B50</f>
         <v>15746.949999999999</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="I18" t="s">
         <v>86</v>
       </c>
-      <c r="I21" t="s">
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D19" t="s">
         <v>75</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E19" t="s">
         <v>88</v>
       </c>
-      <c r="D22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="13">
+      <c r="F19" s="13">
         <f>RBCPriceGenerator!B4</f>
         <v>12822.499999999998</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G19" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I19" t="s">
         <v>91</v>
       </c>
-      <c r="I22" t="s">
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1">
+      <c r="A20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1">
-      <c r="A23" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="D20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="7">
+      <c r="F20" s="7">
         <f>RBCPriceGenerator!B42</f>
         <v>16099.999999999998</v>
       </c>
+      <c r="G20" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="13">
+        <f>RBCPriceGenerator!B24</f>
+        <v>8049.9999999999991</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1">
+      <c r="A22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="4">
+        <f>RBCPriceGenerator!B34</f>
+        <v>10471.9</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="5" customFormat="1" ht="15" thickBot="1">
+      <c r="A23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="7">
+        <f>RBCPriceGenerator!B41</f>
+        <v>8625</v>
+      </c>
       <c r="G23" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" t="s">
-        <v>96</v>
+        <v>103</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1">
@@ -1723,210 +1764,123 @@
         <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
         <v>65</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F24" s="13">
-        <f>RBCPriceGenerator!B32</f>
-        <v>34500</v>
+        <f>RBCPriceGenerator!B28</f>
+        <v>17250</v>
       </c>
       <c r="G24" t="s">
         <v>14</v>
       </c>
+      <c r="H24" s="16" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1">
-      <c r="A25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="13">
-        <f>RBCPriceGenerator!B24</f>
-        <v>8049.9999999999991</v>
-      </c>
-      <c r="G25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1">
-      <c r="A26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="A25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" s="4">
-        <f>RBCPriceGenerator!B34</f>
-        <v>10471.9</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="5" customFormat="1" ht="15" thickBot="1">
-      <c r="A27" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="7">
-        <f>RBCPriceGenerator!B41</f>
-        <v>8625</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1">
-      <c r="A28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="13">
-        <f>RBCPriceGenerator!B28</f>
-        <v>17250</v>
-      </c>
-      <c r="G28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1">
-      <c r="A29" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F25" s="9">
         <f>RBCPriceGenerator!B48</f>
         <v>4401.0499999999993</v>
       </c>
-      <c r="G29" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="H29" s="8" t="s">
+      <c r="G25" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I25" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1">
-      <c r="A30" t="s">
+    <row r="26" spans="1:9" ht="15" thickBot="1">
+      <c r="A26" t="s">
         <v>62</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B26" t="s">
         <v>63</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C26" t="s">
         <v>64</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D26" t="s">
         <v>65</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E26" t="s">
         <v>111</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F26" s="13">
         <f>RBCPriceGenerator!B27</f>
-        <v>24149.999999999996</v>
-      </c>
-      <c r="G30" t="s">
+        <v>65686.849999999991</v>
+      </c>
+      <c r="G26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1">
-      <c r="A31" t="s">
+      <c r="H26" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1">
+      <c r="A27" t="s">
         <v>62</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B27" t="s">
         <v>63</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C27" t="s">
         <v>64</v>
       </c>
-      <c r="D31" t="s">
-        <v>112</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D27" t="s">
         <v>113</v>
       </c>
-      <c r="F31" s="13">
+      <c r="E27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="13">
         <f>RBCPriceGenerator!B23</f>
         <v>5175</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G27" t="s">
         <v>14</v>
       </c>
+      <c r="H27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="F30" s="15"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="F31" s="15"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="F32" s="15"/>
+    </row>
+    <row r="33" spans="6:6">
+      <c r="F33" s="15"/>
     </row>
     <row r="34" spans="6:6">
       <c r="F34" s="15"/>
@@ -1993,15 +1947,19 @@
     </row>
     <row r="55" spans="6:13">
       <c r="F55" s="15"/>
+      <c r="M55" s="15"/>
     </row>
     <row r="56" spans="6:13">
       <c r="F56" s="15"/>
+      <c r="M56" s="15"/>
     </row>
     <row r="57" spans="6:13">
       <c r="F57" s="15"/>
+      <c r="M57" s="15"/>
     </row>
     <row r="58" spans="6:13">
       <c r="F58" s="15"/>
+      <c r="M58" s="15"/>
     </row>
     <row r="59" spans="6:13">
       <c r="F59" s="15"/>
@@ -2020,15 +1978,12 @@
       <c r="M62" s="15"/>
     </row>
     <row r="63" spans="6:13">
-      <c r="F63" s="15"/>
       <c r="M63" s="15"/>
     </row>
     <row r="64" spans="6:13">
-      <c r="F64" s="15"/>
       <c r="M64" s="15"/>
     </row>
     <row r="65" spans="6:13">
-      <c r="F65" s="15"/>
       <c r="M65" s="15"/>
     </row>
     <row r="66" spans="6:13">
@@ -2036,28 +1991,27 @@
       <c r="M66" s="15"/>
     </row>
     <row r="67" spans="6:13">
+      <c r="F67" s="15"/>
       <c r="M67" s="15"/>
     </row>
     <row r="68" spans="6:13">
+      <c r="F68" s="15"/>
       <c r="M68" s="15"/>
     </row>
     <row r="69" spans="6:13">
+      <c r="F69" s="15"/>
       <c r="M69" s="15"/>
     </row>
     <row r="70" spans="6:13">
-      <c r="F70" s="15"/>
       <c r="M70" s="15"/>
     </row>
     <row r="71" spans="6:13">
-      <c r="F71" s="15"/>
       <c r="M71" s="15"/>
     </row>
     <row r="72" spans="6:13">
-      <c r="F72" s="15"/>
       <c r="M72" s="15"/>
     </row>
     <row r="73" spans="6:13">
-      <c r="F73" s="15"/>
       <c r="M73" s="15"/>
     </row>
     <row r="74" spans="6:13">
@@ -2102,34 +2056,22 @@
     <row r="87" spans="13:13">
       <c r="M87" s="15"/>
     </row>
-    <row r="88" spans="13:13">
-      <c r="M88" s="15"/>
-    </row>
-    <row r="89" spans="13:13">
-      <c r="M89" s="15"/>
-    </row>
-    <row r="90" spans="13:13">
-      <c r="M90" s="15"/>
-    </row>
     <row r="91" spans="13:13">
       <c r="M91" s="15"/>
     </row>
-    <row r="95" spans="13:13">
-      <c r="M95" s="15"/>
-    </row>
-    <row r="96" spans="13:13">
-      <c r="M96" s="15"/>
-    </row>
-    <row r="97" spans="13:13">
-      <c r="M97" s="15"/>
-    </row>
-    <row r="98" spans="13:13">
-      <c r="M98" s="15"/>
+    <row r="92" spans="13:13">
+      <c r="M92" s="15"/>
+    </row>
+    <row r="93" spans="13:13">
+      <c r="M93" s="15"/>
+    </row>
+    <row r="94" spans="13:13">
+      <c r="M94" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G31" xr:uid="{01BCF050-2F09-42D0-9049-6BF8B00124F4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G31">
-    <sortCondition descending="1" ref="E14:E31"/>
+  <autoFilter ref="A1:G27" xr:uid="{01BCF050-2F09-42D0-9049-6BF8B00124F4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G27">
+    <sortCondition descending="1" ref="E14:E27"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -2137,9 +2079,11 @@
     <hyperlink ref="I3" r:id="rId2" xr:uid="{52748133-60D7-4085-8A2B-F47A5084AE82}"/>
     <hyperlink ref="I4" r:id="rId3" xr:uid="{C39F7D00-D3EC-4E80-B6DF-FF1AC8554BF2}"/>
     <hyperlink ref="I13" r:id="rId4" xr:uid="{51126B01-EF82-4D3A-A8AC-4C6EDBFD4FA4}"/>
-    <hyperlink ref="H19" r:id="rId5" xr:uid="{64525F2D-8BC7-48E6-883B-74C1E1705D7B}"/>
+    <hyperlink ref="H16" r:id="rId5" xr:uid="{64525F2D-8BC7-48E6-883B-74C1E1705D7B}"/>
     <hyperlink ref="H4" r:id="rId6" xr:uid="{B6E103EA-A26F-4CAE-9611-5E071D398B4B}"/>
     <hyperlink ref="I11" r:id="rId7" xr:uid="{DF7F894D-0311-4E90-BE0A-95CB041C6CAB}"/>
+    <hyperlink ref="H26" r:id="rId8" xr:uid="{7809E0D1-332D-4695-8F3F-ECD6F949564D}"/>
+    <hyperlink ref="H24" r:id="rId9" xr:uid="{D3705807-FC18-484E-B2E9-5B159925D2B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2187,10 +2131,10 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>114</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" hidden="1" thickBot="1">
@@ -2201,13 +2145,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F2" s="13">
         <f>RBCPriceGenerator!B5</f>
@@ -2231,7 +2175,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F3" s="13">
         <f>RBCPriceGenerator!B6</f>
@@ -2321,7 +2265,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -2345,13 +2289,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F8" s="13">
         <f>RBCPriceGenerator!B11</f>
@@ -2369,13 +2313,13 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F9" s="13">
         <f>RBCPriceGenerator!B12</f>
@@ -2417,13 +2361,13 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F11" s="4">
         <f>RBCPriceGenerator!B38</f>
@@ -2441,13 +2385,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F12" s="4">
         <f>RBCPriceGenerator!B39</f>
@@ -2465,13 +2409,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F13" s="4">
         <f>RBCPriceGenerator!B40</f>
@@ -2543,7 +2487,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F16" s="9">
         <f>RBCPriceGenerator!B54</f>
@@ -2564,10 +2508,10 @@
         <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F17" s="13">
         <f>RBCPriceGenerator!B23</f>
@@ -2591,7 +2535,7 @@
         <v>65</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F18" s="13">
         <f>RBCPriceGenerator!B24</f>
@@ -2603,19 +2547,19 @@
     </row>
     <row r="19" spans="1:9" ht="15" hidden="1" thickBot="1">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F19" s="13">
         <f>RBCPriceGenerator!B19</f>
@@ -2627,19 +2571,19 @@
     </row>
     <row r="20" spans="1:9" ht="15" hidden="1" thickBot="1">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F20" s="13">
         <f>RBCPriceGenerator!B20</f>
@@ -2651,50 +2595,50 @@
     </row>
     <row r="21" spans="1:9" ht="15" hidden="1" thickBot="1">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F21" s="13">
         <f>RBCPriceGenerator!B21</f>
         <v>362.25</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" hidden="1" thickBot="1">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E22" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F22" s="13">
         <f>RBCPriceGenerator!B22</f>
         <v>675.05</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" hidden="1" thickBot="1">
@@ -2711,7 +2655,7 @@
         <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F23" s="13">
         <f>RBCPriceGenerator!B25</f>
@@ -2763,7 +2707,7 @@
       </c>
       <c r="F25" s="13">
         <f>RBCPriceGenerator!B27</f>
-        <v>24149.999999999996</v>
+        <v>65686.849999999991</v>
       </c>
       <c r="G25" t="s">
         <v>14</v>
@@ -2774,16 +2718,16 @@
         <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>65</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F26" s="13">
         <f>RBCPriceGenerator!B28</f>
@@ -2798,16 +2742,16 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="F27" s="13">
         <f>RBCPriceGenerator!B29</f>
@@ -2822,16 +2766,16 @@
         <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
         <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F28" s="13">
         <f>RBCPriceGenerator!B30</f>
@@ -2846,16 +2790,16 @@
         <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" t="s">
         <v>70</v>
-      </c>
-      <c r="D29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" t="s">
-        <v>69</v>
       </c>
       <c r="F29" s="13">
         <f>RBCPriceGenerator!B31</f>
@@ -2870,7 +2814,7 @@
         <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
         <v>64</v>
@@ -2879,7 +2823,7 @@
         <v>65</v>
       </c>
       <c r="E30" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="F30" s="13">
         <f>RBCPriceGenerator!B32</f>
@@ -2894,7 +2838,7 @@
         <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
         <v>64</v>
@@ -2903,7 +2847,7 @@
         <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>147</v>
       </c>
       <c r="F31" s="13">
         <f>RBCPriceGenerator!B33</f>
@@ -2915,100 +2859,100 @@
     </row>
     <row r="32" spans="1:9" hidden="1">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F32" s="13">
         <f>RBCPriceGenerator!B2</f>
         <v>4357.3499999999995</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I32" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:9" hidden="1">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
         <v>75</v>
       </c>
-      <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" t="s">
-        <v>77</v>
-      </c>
       <c r="E33" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F33" s="13">
         <f>RBCPriceGenerator!B3</f>
         <v>6899.9999999999991</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I33" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" hidden="1">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="s">
         <v>75</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>88</v>
-      </c>
-      <c r="D34" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" t="s">
-        <v>89</v>
       </c>
       <c r="F34" s="13">
         <f>RBCPriceGenerator!B4</f>
         <v>12822.499999999998</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:9" hidden="1">
       <c r="A35" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="F35" s="4">
         <f>RBCPriceGenerator!B34</f>
@@ -3020,19 +2964,19 @@
     </row>
     <row r="36" spans="1:9" hidden="1">
       <c r="A36" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="E36" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="F36" s="4">
         <f>RBCPriceGenerator!B35</f>
@@ -3042,24 +2986,24 @@
         <v>31</v>
       </c>
       <c r="I36" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:9" hidden="1">
       <c r="A37" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="E37" s="3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="F37" s="4">
         <f>RBCPriceGenerator!B36</f>
@@ -3071,88 +3015,88 @@
     </row>
     <row r="38" spans="1:9" hidden="1">
       <c r="A38" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F38" s="7">
         <f>RBCPriceGenerator!B41</f>
         <v>8625</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:9" hidden="1">
       <c r="A39" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="F39" s="7">
         <f>RBCPriceGenerator!B42</f>
         <v>16099.999999999998</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:9" hidden="1">
       <c r="A40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="D40" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F40" s="9">
         <f>RBCPriceGenerator!B47</f>
         <v>4038.7999999999997</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:9" hidden="1">
       <c r="A41" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>107</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>108</v>
@@ -3162,24 +3106,24 @@
         <v>4401.0499999999993</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:9" hidden="1">
       <c r="A42" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="D42" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="F42" s="9">
         <f>RBCPriceGenerator!B49</f>
@@ -3191,50 +3135,50 @@
     </row>
     <row r="43" spans="1:9" hidden="1">
       <c r="A43" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="D43" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="F43" s="9">
         <f>RBCPriceGenerator!B50</f>
         <v>15746.949999999999</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:9" hidden="1">
       <c r="A44" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="D44" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="E44" s="8" t="s">
         <v>76</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="F44" s="9">
         <f>RBCPriceGenerator!B51</f>
         <v>17480</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="5" customFormat="1" ht="15" hidden="1" thickBot="1">
@@ -3386,23 +3330,23 @@
         <v>27</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F51" s="2">
         <f>RBCPriceGenerator!B67</f>
         <v>35255.549999999996</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" hidden="1" thickBot="1">
@@ -3410,23 +3354,23 @@
         <v>27</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F52" s="2">
         <f>RBCPriceGenerator!B68</f>
         <v>44369.299999999996</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" hidden="1" thickBot="1">
@@ -3434,28 +3378,28 @@
         <v>27</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F53" s="2">
         <f>RBCPriceGenerator!B69</f>
         <v>45158.2</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" hidden="1" thickBot="1">
       <c r="C54" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F54" s="11">
         <f>RBCPriceGenerator!B74</f>
@@ -3506,7 +3450,7 @@
         <v>10471.9</v>
       </c>
       <c r="G60" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -3535,7 +3479,7 @@
         <v>13549.3</v>
       </c>
       <c r="G61" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -3564,7 +3508,7 @@
         <v>15525</v>
       </c>
       <c r="G62" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -3602,7 +3546,7 @@
         <v>10471.9</v>
       </c>
       <c r="G65" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -3631,7 +3575,7 @@
         <v>27098.6</v>
       </c>
       <c r="G66" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -3660,7 +3604,7 @@
         <v>20700</v>
       </c>
       <c r="G67" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -3698,7 +3642,7 @@
         <v>15234.05</v>
       </c>
       <c r="G70" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -3727,7 +3671,7 @@
         <v>26444.249999999996</v>
       </c>
       <c r="G71" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -3756,7 +3700,7 @@
         <v>29071.999999999996</v>
       </c>
       <c r="G72" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3797,7 +3741,7 @@
         <v>15234.05</v>
       </c>
       <c r="G76" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -3826,7 +3770,7 @@
         <v>52888.499999999993</v>
       </c>
       <c r="G77" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -3855,7 +3799,7 @@
         <v>36339.999999999993</v>
       </c>
       <c r="G78" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -3896,7 +3840,7 @@
         <v>41260.85</v>
       </c>
       <c r="G82" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:14">
@@ -3925,7 +3869,7 @@
         <v>52888.499999999993</v>
       </c>
       <c r="G83" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:14">
@@ -3954,7 +3898,7 @@
         <v>36339.999999999993</v>
       </c>
       <c r="G84" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:14">
@@ -3987,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="N85" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="86" spans="1:14">
@@ -4017,7 +3961,7 @@
         <v>0</v>
       </c>
       <c r="N86" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:14">
@@ -4047,7 +3991,7 @@
         <v>0</v>
       </c>
       <c r="N87" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:14">
@@ -4083,7 +4027,7 @@
         <v>41260.85</v>
       </c>
       <c r="G89" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="M89" s="15"/>
     </row>
@@ -4113,7 +4057,7 @@
         <v>52888.499999999993</v>
       </c>
       <c r="G90" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H90">
         <f t="shared" ref="H90:I90" si="23">H$35</f>
@@ -4140,7 +4084,7 @@
         <v>0</v>
       </c>
       <c r="N90" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:14">
@@ -4169,7 +4113,7 @@
         <v>43607.999999999993</v>
       </c>
       <c r="G91" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="H91">
         <f>H$4</f>
@@ -4196,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="N91" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:14">
@@ -4229,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="N92" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:14">
@@ -4267,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="N95" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="96" spans="1:14">
@@ -4296,7 +4240,7 @@
         <v>41260.85</v>
       </c>
       <c r="G96" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H96">
         <f t="shared" ref="H96:K96" si="30">H$7</f>
@@ -4323,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="N96" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="97" spans="1:14">
@@ -4352,7 +4296,7 @@
         <v>79332.749999999985</v>
       </c>
       <c r="G97" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="H97">
         <f t="shared" ref="H97:K97" si="32">H$50</f>
@@ -4379,7 +4323,7 @@
         <v>0</v>
       </c>
       <c r="N97" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -4408,7 +4352,7 @@
         <v>50875.999999999993</v>
       </c>
       <c r="G98" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M98" s="15">
         <f>SUBTOTAL(9,M95:M97)</f>
@@ -4451,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="N101" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="102" spans="1:14">
@@ -4480,7 +4424,7 @@
         <v>0</v>
       </c>
       <c r="N102" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:14">
@@ -4509,7 +4453,7 @@
         <v>0</v>
       </c>
       <c r="N103" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="104" spans="1:14">
@@ -4550,7 +4494,7 @@
         <v>0</v>
       </c>
       <c r="N107" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="108" spans="1:14">
@@ -4579,7 +4523,7 @@
         <v>0</v>
       </c>
       <c r="N108" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="109" spans="1:14">
@@ -4608,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="N109" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="110" spans="1:14">
@@ -4652,7 +4596,7 @@
         <v>0</v>
       </c>
       <c r="N114" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="8:14">
@@ -4681,7 +4625,7 @@
         <v>0</v>
       </c>
       <c r="N115" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="116" spans="8:14">
@@ -4710,7 +4654,7 @@
         <v>0</v>
       </c>
       <c r="N116" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="117" spans="8:14">
@@ -4745,7 +4689,7 @@
         <v>0</v>
       </c>
       <c r="N121" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="122" spans="8:14">
@@ -4774,7 +4718,7 @@
         <v>0</v>
       </c>
       <c r="N122" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="123" spans="8:14">
@@ -4803,7 +4747,7 @@
         <v>0</v>
       </c>
       <c r="N123" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="124" spans="8:14">
@@ -4836,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02EAAD8-D566-4024-B845-4CB318AE8481}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -5103,12 +5047,12 @@
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1">
       <c r="A27" s="14">
-        <f>21000</f>
-        <v>21000</v>
+        <f>57119</f>
+        <v>57119</v>
       </c>
       <c r="B27" s="12">
         <f t="shared" si="0"/>
-        <v>24149.999999999996</v>
+        <v>65686.849999999991</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5573,6 +5517,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100583804D756D08E4CA3423200232226B2" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b3af61a159263512a7f1ce494a3d6b52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="38594f89-c314-49a7-8895-5d17cbb3f834" xmlns:ns3="c062e488-6187-499b-9180-094274b6916e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e65e6323747ef5a712f1b4f0f665253a" ns2:_="" ns3:_="">
     <xsd:import namespace="38594f89-c314-49a7-8895-5d17cbb3f834"/>
@@ -5815,19 +5768,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFB4D44B-BA28-4ECE-9D28-DB5214D251D2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5FDEAF2-72F6-4DE3-BA2B-74A9F9809E88}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5FDEAF2-72F6-4DE3-BA2B-74A9F9809E88}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFB4D44B-BA28-4ECE-9D28-DB5214D251D2}"/>
 </file>
</xml_diff>